<commit_message>
fixing issues found #12 + updating gantt chart
</commit_message>
<xml_diff>
--- a/Compute.Documents/Schedule.xlsx
+++ b/Compute.Documents/Schedule.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14130"/>
@@ -608,7 +608,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="period_selected" max="60" min="1" page="10" val="6"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="period_selected" max="60" min="1" page="10" val="13"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -896,7 +896,7 @@
   <dimension ref="B2:AX40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="W25" sqref="W25"/>
+      <selection activeCell="BJ20" sqref="BJ20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -935,7 +935,7 @@
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
       <c r="N3" s="9">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="O3" s="8"/>
       <c r="Q3" s="10"/>
@@ -1099,7 +1099,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="16">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G9" s="17">
         <v>1</v>
@@ -1126,7 +1126,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="16">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G10" s="17">
         <v>1</v>
@@ -1150,13 +1150,13 @@
         <v>5</v>
       </c>
       <c r="E11" s="16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F11" s="16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G11" s="17">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="V11"/>
       <c r="W11"/>
@@ -1177,13 +1177,13 @@
         <v>5</v>
       </c>
       <c r="E12" s="16">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F12" s="16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G12" s="17">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="V12"/>
       <c r="W12"/>
@@ -1234,10 +1234,10 @@
         <v>1</v>
       </c>
       <c r="F14" s="16">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G14" s="17">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="V14"/>
       <c r="W14"/>
@@ -1258,13 +1258,13 @@
         <v>7</v>
       </c>
       <c r="E15" s="16">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F15" s="16">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G15" s="17">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="V15"/>
       <c r="W15"/>
@@ -1288,10 +1288,10 @@
         <v>0</v>
       </c>
       <c r="F16" s="16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G16" s="17">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="V16"/>
       <c r="W16"/>
@@ -1315,10 +1315,10 @@
         <v>0</v>
       </c>
       <c r="F17" s="16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G17" s="17">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="V17"/>
       <c r="W17"/>
@@ -1342,10 +1342,10 @@
         <v>1</v>
       </c>
       <c r="F18" s="16">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G18" s="17">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="V18"/>
       <c r="W18"/>

</xml_diff>